<commit_message>
version 2 30_12_2020 18_00
se realiza version hasta cargue cabeceras
</commit_message>
<xml_diff>
--- a/CargueMasivoAfiliaciones/Data/Config.xlsx
+++ b/CargueMasivoAfiliaciones/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RPA_Ascension\Documents\CargueMasivoAfiliaciones\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B914AA-B623-4077-A8C8-C7F34CC1959B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F99062A-59FE-4A7B-891D-965B79BFA796}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="11970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="101">
   <si>
     <t>Name</t>
   </si>
@@ -323,6 +323,12 @@
   </si>
   <si>
     <t>Correo</t>
+  </si>
+  <si>
+    <t>C:\Users\RPA_Ascension\Documents\Proyectos\Acension\Formatos</t>
+  </si>
+  <si>
+    <t>RutaSociosNegocios</t>
   </si>
 </sst>
 </file>
@@ -793,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -970,191 +976,198 @@
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B16" t="s">
-        <v>80</v>
+        <v>100</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A18" s="9" t="s">
         <v>98</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A18" s="12" t="s">
-        <v>47</v>
       </c>
       <c r="B18" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A19" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" t="s">
-        <v>46</v>
+      <c r="A19" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A22" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A22" s="10" t="s">
+    <row r="23" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A23" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A23" s="15" t="s">
+    <row r="24" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A24" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A24" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1">
       <c r="A25" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1">
       <c r="A26" s="11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1">
       <c r="A27" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1">
       <c r="A28" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
+      </c>
+      <c r="B28" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1">
       <c r="A29" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1">
       <c r="A30" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1">
       <c r="A31" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1">
       <c r="A32" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
       <c r="A33" s="11" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1">
       <c r="A34" s="11" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
       <c r="A35" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C35" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
       <c r="A36" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>76</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A38" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="39" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A39" s="11" t="s">
+    <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A40" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="41" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2112,6 +2125,7 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
+    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
se agrega nueva infomacion
cabeceras ajustes con numero de contrato
</commit_message>
<xml_diff>
--- a/CargueMasivoAfiliaciones/Data/Config.xlsx
+++ b/CargueMasivoAfiliaciones/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RPA_Ascension\Documents\CargueMasivoAfiliaciones\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F99062A-59FE-4A7B-891D-965B79BFA796}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C87C75F-CD02-45B5-880C-E0483C5A6954}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="11970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -802,7 +802,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>